<commit_message>
plots for 2000 accross basline and carbon tax
</commit_message>
<xml_diff>
--- a/report_2000.xlsx
+++ b/report_2000.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:AC77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,66 @@
           <t>SD EOD 3</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Generator Output EOD 4</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Committment Status EOD 4</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>SU EOD 4</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>SD EOD 4</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Generator Output EOD 5</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Committment Status EOD 5</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>SU EOD 5</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>SD EOD 5</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Generator Output EOD 6</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Committment Status EOD 6</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>SU EOD 6</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>SD EOD 6</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -567,6 +627,42 @@
       <c r="Q2" t="n">
         <v>0</v>
       </c>
+      <c r="R2" t="n">
+        <v>1244</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1244</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1244</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -618,6 +714,42 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1235</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1235</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1235</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -673,6 +805,42 @@
       <c r="Q4" t="n">
         <v>0</v>
       </c>
+      <c r="R4" t="n">
+        <v>881</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>881</v>
+      </c>
+      <c r="W4" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>881</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -726,6 +894,42 @@
       <c r="Q5" t="n">
         <v>0</v>
       </c>
+      <c r="R5" t="n">
+        <v>684.7</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>684.7</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>684.7</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -779,6 +983,42 @@
       <c r="Q6" t="n">
         <v>0</v>
       </c>
+      <c r="R6" t="n">
+        <v>620.2</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>620.2</v>
+      </c>
+      <c r="W6" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>620.2</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -832,6 +1072,42 @@
       <c r="Q7" t="n">
         <v>0</v>
       </c>
+      <c r="R7" t="n">
+        <v>612</v>
+      </c>
+      <c r="S7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>612</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>612</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -885,6 +1161,42 @@
       <c r="Q8" t="n">
         <v>0</v>
       </c>
+      <c r="R8" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -938,6 +1250,42 @@
       <c r="Q9" t="n">
         <v>0</v>
       </c>
+      <c r="R9" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="W9" t="n">
+        <v>1</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>372.2</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -991,6 +1339,42 @@
       <c r="Q10" t="n">
         <v>0</v>
       </c>
+      <c r="R10" t="n">
+        <v>244</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>244</v>
+      </c>
+      <c r="W10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>244</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1044,6 +1428,42 @@
       <c r="Q11" t="n">
         <v>0</v>
       </c>
+      <c r="R11" t="n">
+        <v>243.5</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>243.5</v>
+      </c>
+      <c r="W11" t="n">
+        <v>1</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>243.5</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1097,6 +1517,42 @@
       <c r="Q12" t="n">
         <v>0</v>
       </c>
+      <c r="R12" t="n">
+        <v>149.8</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" t="n">
+        <v>149.8</v>
+      </c>
+      <c r="W12" t="n">
+        <v>1</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>149.8</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1150,6 +1606,42 @@
       <c r="Q13" t="n">
         <v>0</v>
       </c>
+      <c r="R13" t="n">
+        <v>144.4</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>144.4</v>
+      </c>
+      <c r="W13" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>144.4</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1203,6 +1695,42 @@
       <c r="Q14" t="n">
         <v>0</v>
       </c>
+      <c r="R14" t="n">
+        <v>82</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" t="n">
+        <v>82</v>
+      </c>
+      <c r="W14" t="n">
+        <v>1</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>82</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1256,6 +1784,42 @@
       <c r="Q15" t="n">
         <v>0</v>
       </c>
+      <c r="R15" t="n">
+        <v>80</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>80</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>80</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1309,6 +1873,42 @@
       <c r="Q16" t="n">
         <v>0</v>
       </c>
+      <c r="R16" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="W16" t="n">
+        <v>1</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1362,6 +1962,42 @@
       <c r="Q17" t="n">
         <v>0</v>
       </c>
+      <c r="R17" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="W17" t="n">
+        <v>1</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1415,6 +2051,42 @@
       <c r="Q18" t="n">
         <v>0</v>
       </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1468,6 +2140,42 @@
       <c r="Q19" t="n">
         <v>0</v>
       </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1521,6 +2229,42 @@
       <c r="Q20" t="n">
         <v>0</v>
       </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1574,6 +2318,42 @@
       <c r="Q21" t="n">
         <v>0</v>
       </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1627,6 +2407,42 @@
       <c r="Q22" t="n">
         <v>0</v>
       </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1680,6 +2496,42 @@
       <c r="Q23" t="n">
         <v>0</v>
       </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
+      <c r="U23" t="n">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1733,6 +2585,42 @@
       <c r="Q24" t="n">
         <v>0</v>
       </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1786,6 +2674,42 @@
       <c r="Q25" t="n">
         <v>3</v>
       </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="n">
+        <v>4</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1839,6 +2763,42 @@
       <c r="Q26" t="n">
         <v>0</v>
       </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1892,6 +2852,42 @@
       <c r="Q27" t="n">
         <v>0</v>
       </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1945,6 +2941,42 @@
       <c r="Q28" t="n">
         <v>0</v>
       </c>
+      <c r="R28" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" t="n">
+        <v>2</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1998,6 +3030,42 @@
       <c r="Q29" t="n">
         <v>0</v>
       </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>4</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2051,6 +3119,42 @@
       <c r="Q30" t="n">
         <v>0</v>
       </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2104,6 +3208,42 @@
       <c r="Q31" t="n">
         <v>0</v>
       </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2157,6 +3297,42 @@
       <c r="Q32" t="n">
         <v>0</v>
       </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
+        <v>11</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2210,6 +3386,42 @@
       <c r="Q33" t="n">
         <v>0</v>
       </c>
+      <c r="R33" t="n">
+        <v>693.8</v>
+      </c>
+      <c r="S33" t="n">
+        <v>1</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>693.8</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>693.8</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2263,6 +3475,42 @@
       <c r="Q34" t="n">
         <v>0</v>
       </c>
+      <c r="R34" t="n">
+        <v>685.3</v>
+      </c>
+      <c r="S34" t="n">
+        <v>1</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" t="n">
+        <v>685.3</v>
+      </c>
+      <c r="W34" t="n">
+        <v>1</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>685.3</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2316,6 +3564,42 @@
       <c r="Q35" t="n">
         <v>11</v>
       </c>
+      <c r="R35" t="n">
+        <v>438.078622</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2369,6 +3653,42 @@
       <c r="Q36" t="n">
         <v>0</v>
       </c>
+      <c r="R36" t="n">
+        <v>110.9599999999999</v>
+      </c>
+      <c r="S36" t="n">
+        <v>1</v>
+      </c>
+      <c r="T36" t="n">
+        <v>7</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>110.96</v>
+      </c>
+      <c r="W36" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>110.96</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2422,6 +3742,42 @@
       <c r="Q37" t="n">
         <v>0</v>
       </c>
+      <c r="R37" t="n">
+        <v>515.5</v>
+      </c>
+      <c r="S37" t="n">
+        <v>1</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>515.5</v>
+      </c>
+      <c r="W37" t="n">
+        <v>1</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>515.5</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2475,6 +3831,42 @@
       <c r="Q38" t="n">
         <v>0</v>
       </c>
+      <c r="R38" t="n">
+        <v>508</v>
+      </c>
+      <c r="S38" t="n">
+        <v>1</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>508</v>
+      </c>
+      <c r="W38" t="n">
+        <v>1</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>508</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2528,6 +3920,42 @@
       <c r="Q39" t="n">
         <v>0</v>
       </c>
+      <c r="R39" t="n">
+        <v>490.4</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>490.4</v>
+      </c>
+      <c r="W39" t="n">
+        <v>1</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>490.4</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2581,6 +4009,42 @@
       <c r="Q40" t="n">
         <v>0</v>
       </c>
+      <c r="R40" t="n">
+        <v>447.9</v>
+      </c>
+      <c r="S40" t="n">
+        <v>1</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="n">
+        <v>1</v>
+      </c>
+      <c r="V40" t="n">
+        <v>432.2194689189191</v>
+      </c>
+      <c r="W40" t="n">
+        <v>1</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>447.9</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2634,6 +4098,42 @@
       <c r="Q41" t="n">
         <v>0</v>
       </c>
+      <c r="R41" t="n">
+        <v>270.9</v>
+      </c>
+      <c r="S41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="n">
+        <v>0</v>
+      </c>
+      <c r="V41" t="n">
+        <v>270.9</v>
+      </c>
+      <c r="W41" t="n">
+        <v>1</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>270.9</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2687,6 +4187,42 @@
       <c r="Q42" t="n">
         <v>5</v>
       </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="n">
+        <v>5</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="n">
+        <v>0</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2740,6 +4276,42 @@
       <c r="Q43" t="n">
         <v>0</v>
       </c>
+      <c r="R43" t="n">
+        <v>248.7</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1</v>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
+      </c>
+      <c r="U43" t="n">
+        <v>0</v>
+      </c>
+      <c r="V43" t="n">
+        <v>248.7</v>
+      </c>
+      <c r="W43" t="n">
+        <v>1</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>248.7</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2793,6 +4365,42 @@
       <c r="Q44" t="n">
         <v>0</v>
       </c>
+      <c r="R44" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="S44" t="n">
+        <v>1</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="W44" t="n">
+        <v>1</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2846,6 +4454,42 @@
       <c r="Q45" t="n">
         <v>0</v>
       </c>
+      <c r="R45" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="S45" t="n">
+        <v>1</v>
+      </c>
+      <c r="T45" t="n">
+        <v>0</v>
+      </c>
+      <c r="U45" t="n">
+        <v>0</v>
+      </c>
+      <c r="V45" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="W45" t="n">
+        <v>1</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>247.8</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2899,6 +4543,42 @@
       <c r="Q46" t="n">
         <v>0</v>
       </c>
+      <c r="R46" t="n">
+        <v>244.9</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T46" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" t="n">
+        <v>0</v>
+      </c>
+      <c r="V46" t="n">
+        <v>87.36028308108155</v>
+      </c>
+      <c r="W46" t="n">
+        <v>1</v>
+      </c>
+      <c r="X46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>244.9</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2952,6 +4632,42 @@
       <c r="Q47" t="n">
         <v>6</v>
       </c>
+      <c r="R47" t="n">
+        <v>0</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0</v>
+      </c>
+      <c r="U47" t="n">
+        <v>6</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0</v>
+      </c>
+      <c r="X47" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -3005,6 +4721,42 @@
       <c r="Q48" t="n">
         <v>4</v>
       </c>
+      <c r="R48" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="n">
+        <v>5</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="n">
+        <v>0</v>
+      </c>
+      <c r="X48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -3058,6 +4810,42 @@
       <c r="Q49" t="n">
         <v>0</v>
       </c>
+      <c r="R49" t="n">
+        <v>238.3</v>
+      </c>
+      <c r="S49" t="n">
+        <v>1</v>
+      </c>
+      <c r="T49" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" t="n">
+        <v>0</v>
+      </c>
+      <c r="V49" t="n">
+        <v>238.3</v>
+      </c>
+      <c r="W49" t="n">
+        <v>1</v>
+      </c>
+      <c r="X49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>238.3</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -3111,6 +4899,42 @@
       <c r="Q50" t="n">
         <v>0</v>
       </c>
+      <c r="R50" t="n">
+        <v>0</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0</v>
+      </c>
+      <c r="T50" t="n">
+        <v>0</v>
+      </c>
+      <c r="U50" t="n">
+        <v>5</v>
+      </c>
+      <c r="V50" t="n">
+        <v>0</v>
+      </c>
+      <c r="W50" t="n">
+        <v>0</v>
+      </c>
+      <c r="X50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB50" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -3164,6 +4988,42 @@
       <c r="Q51" t="n">
         <v>0</v>
       </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>0</v>
+      </c>
+      <c r="T51" t="n">
+        <v>0</v>
+      </c>
+      <c r="U51" t="n">
+        <v>10</v>
+      </c>
+      <c r="V51" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="W51" t="n">
+        <v>1</v>
+      </c>
+      <c r="X51" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>30.93999999999991</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB51" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -3217,6 +5077,42 @@
       <c r="Q52" t="n">
         <v>5</v>
       </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0</v>
+      </c>
+      <c r="U52" t="n">
+        <v>5</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC52" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -3270,6 +5166,42 @@
       <c r="Q53" t="n">
         <v>5</v>
       </c>
+      <c r="R53" t="n">
+        <v>0</v>
+      </c>
+      <c r="S53" t="n">
+        <v>0</v>
+      </c>
+      <c r="T53" t="n">
+        <v>0</v>
+      </c>
+      <c r="U53" t="n">
+        <v>4</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0</v>
+      </c>
+      <c r="X53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB53" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC53" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3323,6 +5255,42 @@
       <c r="Q54" t="n">
         <v>4</v>
       </c>
+      <c r="R54" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0</v>
+      </c>
+      <c r="T54" t="n">
+        <v>0</v>
+      </c>
+      <c r="U54" t="n">
+        <v>4</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB54" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC54" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3376,6 +5344,42 @@
       <c r="Q55" t="n">
         <v>3</v>
       </c>
+      <c r="R55" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0</v>
+      </c>
+      <c r="T55" t="n">
+        <v>0</v>
+      </c>
+      <c r="U55" t="n">
+        <v>4</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB55" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC55" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3429,6 +5433,42 @@
       <c r="Q56" t="n">
         <v>3</v>
       </c>
+      <c r="R56" t="n">
+        <v>0</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0</v>
+      </c>
+      <c r="U56" t="n">
+        <v>3</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB56" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC56" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3482,6 +5522,42 @@
       <c r="Q57" t="n">
         <v>0</v>
       </c>
+      <c r="R57" t="n">
+        <v>0</v>
+      </c>
+      <c r="S57" t="n">
+        <v>0</v>
+      </c>
+      <c r="T57" t="n">
+        <v>0</v>
+      </c>
+      <c r="U57" t="n">
+        <v>0</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB57" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3535,6 +5611,42 @@
       <c r="Q58" t="n">
         <v>5</v>
       </c>
+      <c r="R58" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" t="n">
+        <v>0</v>
+      </c>
+      <c r="U58" t="n">
+        <v>6</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0</v>
+      </c>
+      <c r="W58" t="n">
+        <v>0</v>
+      </c>
+      <c r="X58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC58" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3588,6 +5700,42 @@
       <c r="Q59" t="n">
         <v>0</v>
       </c>
+      <c r="R59" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="n">
+        <v>0</v>
+      </c>
+      <c r="T59" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="n">
+        <v>3</v>
+      </c>
+      <c r="V59" t="n">
+        <v>0</v>
+      </c>
+      <c r="W59" t="n">
+        <v>0</v>
+      </c>
+      <c r="X59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3641,6 +5789,42 @@
       <c r="Q60" t="n">
         <v>0</v>
       </c>
+      <c r="R60" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="n">
+        <v>0</v>
+      </c>
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="n">
+        <v>0</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0</v>
+      </c>
+      <c r="X60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB60" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3694,6 +5878,42 @@
       <c r="Q61" t="n">
         <v>0</v>
       </c>
+      <c r="R61" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="n">
+        <v>0</v>
+      </c>
+      <c r="T61" t="n">
+        <v>0</v>
+      </c>
+      <c r="U61" t="n">
+        <v>0</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" t="n">
+        <v>0</v>
+      </c>
+      <c r="X61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB61" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3747,6 +5967,42 @@
       <c r="Q62" t="n">
         <v>0</v>
       </c>
+      <c r="R62" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="n">
+        <v>0</v>
+      </c>
+      <c r="T62" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" t="n">
+        <v>0</v>
+      </c>
+      <c r="V62" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" t="n">
+        <v>0</v>
+      </c>
+      <c r="X62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3800,6 +6056,42 @@
       <c r="Q63" t="n">
         <v>0</v>
       </c>
+      <c r="R63" t="n">
+        <v>0</v>
+      </c>
+      <c r="S63" t="n">
+        <v>0</v>
+      </c>
+      <c r="T63" t="n">
+        <v>0</v>
+      </c>
+      <c r="U63" t="n">
+        <v>0</v>
+      </c>
+      <c r="V63" t="n">
+        <v>0</v>
+      </c>
+      <c r="W63" t="n">
+        <v>0</v>
+      </c>
+      <c r="X63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB63" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3853,6 +6145,42 @@
       <c r="Q64" t="n">
         <v>0</v>
       </c>
+      <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T64" t="n">
+        <v>0</v>
+      </c>
+      <c r="U64" t="n">
+        <v>0</v>
+      </c>
+      <c r="V64" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="n">
+        <v>0</v>
+      </c>
+      <c r="X64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3906,6 +6234,42 @@
       <c r="Q65" t="n">
         <v>0</v>
       </c>
+      <c r="R65" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" t="n">
+        <v>0</v>
+      </c>
+      <c r="T65" t="n">
+        <v>0</v>
+      </c>
+      <c r="U65" t="n">
+        <v>0</v>
+      </c>
+      <c r="V65" t="n">
+        <v>0</v>
+      </c>
+      <c r="W65" t="n">
+        <v>0</v>
+      </c>
+      <c r="X65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3959,6 +6323,42 @@
       <c r="Q66" t="n">
         <v>0</v>
       </c>
+      <c r="R66" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" t="n">
+        <v>0</v>
+      </c>
+      <c r="U66" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -4012,6 +6412,42 @@
       <c r="Q67" t="n">
         <v>0</v>
       </c>
+      <c r="R67" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="n">
+        <v>0</v>
+      </c>
+      <c r="T67" t="n">
+        <v>0</v>
+      </c>
+      <c r="U67" t="n">
+        <v>0</v>
+      </c>
+      <c r="V67" t="n">
+        <v>0</v>
+      </c>
+      <c r="W67" t="n">
+        <v>0</v>
+      </c>
+      <c r="X67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -4065,6 +6501,42 @@
       <c r="Q68" t="n">
         <v>0</v>
       </c>
+      <c r="R68" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="n">
+        <v>0</v>
+      </c>
+      <c r="T68" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="n">
+        <v>0</v>
+      </c>
+      <c r="X68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -4118,6 +6590,42 @@
       <c r="Q69" t="n">
         <v>0</v>
       </c>
+      <c r="R69" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="n">
+        <v>0</v>
+      </c>
+      <c r="T69" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="n">
+        <v>0</v>
+      </c>
+      <c r="V69" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="n">
+        <v>0</v>
+      </c>
+      <c r="X69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB69" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -4171,6 +6679,42 @@
       <c r="Q70" t="n">
         <v>0</v>
       </c>
+      <c r="R70" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" t="n">
+        <v>0</v>
+      </c>
+      <c r="U70" t="n">
+        <v>0</v>
+      </c>
+      <c r="V70" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="n">
+        <v>0</v>
+      </c>
+      <c r="X70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -4224,6 +6768,42 @@
       <c r="Q71" t="n">
         <v>0</v>
       </c>
+      <c r="R71" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="n">
+        <v>0</v>
+      </c>
+      <c r="T71" t="n">
+        <v>0</v>
+      </c>
+      <c r="U71" t="n">
+        <v>0</v>
+      </c>
+      <c r="V71" t="n">
+        <v>0</v>
+      </c>
+      <c r="W71" t="n">
+        <v>0</v>
+      </c>
+      <c r="X71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -4277,6 +6857,42 @@
       <c r="Q72" t="n">
         <v>0</v>
       </c>
+      <c r="R72" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="n">
+        <v>0</v>
+      </c>
+      <c r="T72" t="n">
+        <v>0</v>
+      </c>
+      <c r="U72" t="n">
+        <v>0</v>
+      </c>
+      <c r="V72" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="n">
+        <v>0</v>
+      </c>
+      <c r="X72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -4330,6 +6946,42 @@
       <c r="Q73" t="n">
         <v>0</v>
       </c>
+      <c r="R73" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="n">
+        <v>0</v>
+      </c>
+      <c r="T73" t="n">
+        <v>0</v>
+      </c>
+      <c r="U73" t="n">
+        <v>0</v>
+      </c>
+      <c r="V73" t="n">
+        <v>0</v>
+      </c>
+      <c r="W73" t="n">
+        <v>0</v>
+      </c>
+      <c r="X73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -4383,6 +7035,42 @@
       <c r="Q74" t="n">
         <v>0</v>
       </c>
+      <c r="R74" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="n">
+        <v>0</v>
+      </c>
+      <c r="X74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -4436,6 +7124,42 @@
       <c r="Q75" t="n">
         <v>0</v>
       </c>
+      <c r="R75" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" t="n">
+        <v>0</v>
+      </c>
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="n">
+        <v>0</v>
+      </c>
+      <c r="X75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -4489,6 +7213,42 @@
       <c r="Q76" t="n">
         <v>0</v>
       </c>
+      <c r="R76" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="n">
+        <v>0</v>
+      </c>
+      <c r="T76" t="n">
+        <v>0</v>
+      </c>
+      <c r="U76" t="n">
+        <v>0</v>
+      </c>
+      <c r="V76" t="n">
+        <v>0</v>
+      </c>
+      <c r="W76" t="n">
+        <v>0</v>
+      </c>
+      <c r="X76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -4540,6 +7300,42 @@
         <v>0</v>
       </c>
       <c r="Q77" t="n">
+        <v>0</v>
+      </c>
+      <c r="R77" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="n">
+        <v>0</v>
+      </c>
+      <c r="T77" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" t="n">
+        <v>0</v>
+      </c>
+      <c r="V77" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="n">
+        <v>0</v>
+      </c>
+      <c r="X77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>